<commit_message>
updated stm kinetic input files
</commit_message>
<xml_diff>
--- a/data/stm_kinetic/MMP11_stm.xlsx
+++ b/data/stm_kinetic/MMP11_stm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariaalonso/Work/protease_activity_analysis/protease_activity_analysis/tests/data/stm_kinetic/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariaalonso/Work/protease_activity_analysis/data/stm_kinetic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61817B50-C7F8-8943-AF2B-47B28DA8CF69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFB7FBD-26D7-C14B-8376-1F5C87E55E37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="1740" windowWidth="27640" windowHeight="16120" xr2:uid="{CECF4070-B571-CF4F-96AF-45B2DF00BB8B}"/>
+    <workbookView xWindow="860" yWindow="860" windowWidth="27640" windowHeight="16120" xr2:uid="{CECF4070-B571-CF4F-96AF-45B2DF00BB8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -426,7 +426,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66CCA8A1-CB95-4644-AEDC-6E4EC98E6FDD}">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -495,7 +497,7 @@
         <v>37</v>
       </c>
       <c r="V1">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>